<commit_message>
working except for expoert
</commit_message>
<xml_diff>
--- a/data/model-infos/updated-sustainability/artificial class information.xlsx
+++ b/data/model-infos/updated-sustainability/artificial class information.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexholland/Coding/tree-sim/data/model-infos/updated-sustainability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{36C9DDC0-543C-414D-8BF1-CB2884A8AE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC9019F-8C81-D345-A79C-61A48DF11D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="11380" windowWidth="31600" windowHeight="19200" activeTab="2"/>
+    <workbookView xWindow="-31580" yWindow="5740" windowWidth="31600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="artificial stats" sheetId="1" r:id="rId1"/>
     <sheet name="snag measures" sheetId="2" r:id="rId2"/>
     <sheet name="snag distributions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>no</t>
   </si>
@@ -42,15 +55,6 @@
     <t>snag</t>
   </si>
   <si>
-    <t>5-pole</t>
-  </si>
-  <si>
-    <t>4-pole</t>
-  </si>
-  <si>
-    <t>6-snag</t>
-  </si>
-  <si>
     <t>perch</t>
   </si>
   <si>
@@ -60,12 +64,6 @@
     <t>perchHigh</t>
   </si>
   <si>
-    <t>lifeLow</t>
-  </si>
-  <si>
-    <t>lifeHigh</t>
-  </si>
-  <si>
     <t>costLow</t>
   </si>
   <si>
@@ -112,12 +110,81 @@
   </si>
   <si>
     <t>resource</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>Use trees</t>
+  </si>
+  <si>
+    <t>Use trees, maintain trees, and renew trees in cycles</t>
+  </si>
+  <si>
+    <t>Use trees, maintain trees, renew trees, and source cheaply</t>
+  </si>
+  <si>
+    <t>Use poles</t>
+  </si>
+  <si>
+    <t>Use poles, source as cheaply as possible</t>
+  </si>
+  <si>
+    <t>Use snags</t>
+  </si>
+  <si>
+    <t>Use snags but retain branches</t>
+  </si>
+  <si>
+    <t>Use snags, retain branches, and source cheaply</t>
+  </si>
+  <si>
+    <t>Baseline woodland</t>
+  </si>
+  <si>
+    <t>weighted snag cost</t>
+  </si>
+  <si>
+    <t>weighted tree costs</t>
+  </si>
+  <si>
+    <t>weighted pole costs</t>
+  </si>
+  <si>
+    <t>weighting</t>
+  </si>
+  <si>
+    <t>variation</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>the weighted value becomes the high end of costs so snag cost selected from low end of range to match scenario 8</t>
+  </si>
+  <si>
+    <t>isArtificials</t>
+  </si>
+  <si>
+    <t>isExistingTrees</t>
+  </si>
+  <si>
+    <t>isRecruit</t>
+  </si>
+  <si>
+    <t>serviceLife</t>
+  </si>
+  <si>
+    <t>weighted low</t>
+  </si>
+  <si>
+    <t>weighted high</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="26">
     <font>
       <sz val="12"/>
@@ -655,12 +722,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1015,16 +1082,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="51.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1032,311 +1102,653 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>J3-E15</f>
+        <v>115.2</v>
+      </c>
+      <c r="J3">
+        <v>144</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>J3-E15</f>
+        <v>115.2</v>
+      </c>
+      <c r="J4">
+        <v>144</v>
+      </c>
+      <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>72</v>
+      </c>
+      <c r="J5">
+        <f>I5+E16</f>
+        <v>86.4</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>12.603391999999999</v>
+      </c>
+      <c r="E6">
+        <v>15.754239999999999</v>
+      </c>
+      <c r="F6">
+        <v>2.6033751999999999</v>
+      </c>
+      <c r="G6">
+        <v>3.254219</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>1524.06</v>
+      </c>
+      <c r="J6">
+        <v>16815</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>12.603391999999999</v>
+      </c>
+      <c r="E7">
+        <v>15.754239999999999</v>
+      </c>
+      <c r="F7">
+        <v>2.6033751999999999</v>
+      </c>
+      <c r="G7">
+        <v>3.254219</v>
+      </c>
+      <c r="H7">
+        <v>25</v>
+      </c>
+      <c r="I7">
+        <v>1524.06</v>
+      </c>
+      <c r="J7">
+        <v>2243.3200000000002</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="I8">
+        <v>12147</v>
+      </c>
+      <c r="J8">
+        <v>24294</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
-        <v>12.603391999999999</v>
-      </c>
-      <c r="E2" s="2">
-        <v>15.754239999999999</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2.6033751999999999</v>
-      </c>
-      <c r="G2" s="2">
-        <v>3.254219</v>
-      </c>
-      <c r="H2">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>25</v>
       </c>
-      <c r="I2">
+      <c r="I9">
+        <v>12147</v>
+      </c>
+      <c r="J9">
+        <v>24294</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>25</v>
       </c>
-      <c r="J2" s="3">
-        <v>1524.06</v>
-      </c>
-      <c r="K2">
-        <v>16815</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>12.603391999999999</v>
-      </c>
-      <c r="E3" s="2">
-        <v>15.754239999999999</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2.6033751999999999</v>
-      </c>
-      <c r="G3" s="2">
-        <v>3.254219</v>
-      </c>
-      <c r="H3">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1524.06</v>
-      </c>
-      <c r="K3" s="3">
-        <v>2243.3200000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>51.777019000000003</v>
-      </c>
-      <c r="E4">
-        <v>130.556532</v>
-      </c>
-      <c r="F4" s="2">
-        <v>9.6660740000000001</v>
-      </c>
-      <c r="G4" s="2">
-        <v>43.227826999999998</v>
-      </c>
-      <c r="H4">
-        <v>25</v>
-      </c>
-      <c r="I4">
-        <v>25</v>
-      </c>
-      <c r="J4">
+      <c r="I10">
         <v>12147</v>
       </c>
-      <c r="K4">
-        <v>24294</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="G6" s="2"/>
+      <c r="J10">
+        <f>F17</f>
+        <v>14576.4</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>144</v>
+      </c>
+      <c r="E15">
+        <f>D20*D15</f>
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="D16">
+        <v>72</v>
+      </c>
+      <c r="E16">
+        <f>D16*D20</f>
+        <v>14.4</v>
+      </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <f>I8</f>
+        <v>12147</v>
+      </c>
+      <c r="E17">
+        <f>D17*$D$20</f>
+        <v>2429.4</v>
+      </c>
+      <c r="F17">
+        <f>D17+E17</f>
+        <v>14576.4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="1:14">
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="M18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="D21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>0.2</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="M20" s="3"/>
     </row>
     <row r="22" spans="1:14">
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:14">
       <c r="D23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="C25" s="2"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:14">
       <c r="C26" s="2"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="C27" s="2"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:14">
       <c r="C28" s="2"/>
-      <c r="I28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" t="s">
-        <v>22</v>
-      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" t="s">
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="C30" s="2"/>
+      <c r="I30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
         <v>3</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G31" t="s">
         <v>1</v>
       </c>
-      <c r="I29">
-        <f>MEDIAN(B31:B33)</f>
+      <c r="I31">
+        <f>MEDIAN(B33:B35)</f>
         <v>53.415900000000001</v>
       </c>
-      <c r="J29">
-        <f>_xlfn.STDEV.S(B31:B33)</f>
+      <c r="J31">
+        <f>_xlfn.STDEV.S(B33:B35)</f>
         <v>45.017725990790588</v>
       </c>
-      <c r="K29">
-        <f>I29-2*J29</f>
+      <c r="K31">
+        <f>I31-2*J31</f>
         <v>-36.619551981581175</v>
       </c>
-      <c r="L29">
-        <f>MEDIAN(I29+2*J29)</f>
+      <c r="L31">
+        <f>MEDIAN(I31+2*J31)</f>
         <v>143.45135198158118</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="6">
+    <row r="32" spans="1:14">
+      <c r="A32" s="5">
         <v>4</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B32" s="5">
         <v>15.754239999999999</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C32" s="5">
         <v>3.254219</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="6">
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="5">
         <v>1</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B33" s="5">
         <v>130.55653000000001</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C33" s="5">
         <v>43.227826999999998</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="6">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="5">
         <v>2</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B34" s="5">
         <v>51.77702</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C34" s="5">
         <v>9.6660740000000001</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="7">
+    <row r="35" spans="1:10">
+      <c r="A35" s="6">
         <v>3</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B35" s="6">
         <v>53.415900000000001</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C35" s="6">
         <v>11.303186999999999</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="B12:E13"/>
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1346,7 +1758,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1354,110 +1766,110 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>15.754239999999999</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>3.254219</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>130.55653000000001</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>43.227826999999998</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>51.77702</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>9.6660740000000001</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>53.415900000000001</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>11.303186999999999</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="10">
+        <v>13</v>
+      </c>
+      <c r="B10" s="9">
         <f>GEOMEAN(B4:B6)</f>
         <v>71.209084126764083</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <f>STDEV(B4:B6)</f>
         <v>45.017725990790588</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>-36.619551999999999</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>143.45135200000001</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <f>GEOMEAN(C4:C6)</f>
@@ -1476,18 +1888,18 @@
         <v>54.621934519385839</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="10">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9">
         <f>B10</f>
         <v>71.209084126764083</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f>C10</f>
         <v>45.017725990790588</v>
       </c>
@@ -1502,7 +1914,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <f>B11</f>
@@ -1512,7 +1924,7 @@
         <f>C11</f>
         <v>18.922006775786134</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f>C5</f>
         <v>9.6660740000000001</v>
       </c>
@@ -1522,8 +1934,8 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="8"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1531,11 +1943,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1545,24 +1957,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>71.209084126764083</v>
@@ -1579,7 +1991,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>16.777920967813571</v>

</xml_diff>

<commit_message>
final, added gitignores to output folders
</commit_message>
<xml_diff>
--- a/data/model-infos/updated-sustainability/artificial class information.xlsx
+++ b/data/model-infos/updated-sustainability/artificial class information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexholland/Coding/tree-sim/data/model-infos/updated-sustainability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC9019F-8C81-D345-A79C-61A48DF11D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB42BF9-2262-5D40-889B-FA633E2AAF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31580" yWindow="5740" windowWidth="31600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31600" yWindow="7500" windowWidth="31600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="artificial stats" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>no</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>weighted high</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>treeDeathLow</t>
+  </si>
+  <si>
+    <t>treeDeathHigh</t>
   </si>
 </sst>
 </file>
@@ -1083,18 +1092,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="51.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1105,37 +1115,46 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1146,7 +1165,7 @@
         <v>34</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1166,17 +1185,26 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2" t="b">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
       <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="O2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1187,7 +1215,7 @@
         <v>26</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1202,23 +1230,32 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f>J3-E15</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>K3-F15</f>
         <v>115.2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>144</v>
       </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
       <c r="L3" t="b">
         <v>0</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P3">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1229,7 +1266,7 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1244,23 +1281,32 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f>J3-E15</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>K3-F15</f>
         <v>115.2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>144</v>
       </c>
-      <c r="K4" t="b">
+      <c r="L4" t="b">
         <v>1</v>
       </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
       <c r="M4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1271,7 +1317,7 @@
         <v>28</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1286,23 +1332,32 @@
         <v>0</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>72</v>
       </c>
-      <c r="J5">
-        <f>I5+E16</f>
+      <c r="K5">
+        <f>J5+F16</f>
         <v>86.4</v>
       </c>
-      <c r="K5" t="b">
+      <c r="L5" t="b">
         <v>1</v>
       </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
       <c r="M5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1313,37 +1368,46 @@
         <v>29</v>
       </c>
       <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
         <v>12.603391999999999</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>15.754239999999999</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2.6033751999999999</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>3.254219</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>25</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1524.06</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>16815</v>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
       </c>
       <c r="M6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1354,37 +1418,46 @@
         <v>30</v>
       </c>
       <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
         <v>12.603391999999999</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>15.754239999999999</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2.6033751999999999</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3.254219</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>25</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1524.06</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2243.3200000000002</v>
-      </c>
-      <c r="K7" t="b">
-        <v>1</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
       </c>
       <c r="M7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1395,7 +1468,7 @@
         <v>31</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1407,25 +1480,34 @@
         <v>0</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>25</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>12147</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>24294</v>
-      </c>
-      <c r="K8" t="b">
-        <v>1</v>
       </c>
       <c r="L8" t="b">
         <v>1</v>
       </c>
       <c r="M8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1436,7 +1518,7 @@
         <v>32</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1448,25 +1530,34 @@
         <v>0</v>
       </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>25</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>12147</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>24294</v>
-      </c>
-      <c r="K9" t="b">
-        <v>1</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
       </c>
       <c r="M9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>1</v>
+      </c>
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1477,7 +1568,7 @@
         <v>33</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1489,160 +1580,175 @@
         <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>25</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>12147</v>
       </c>
-      <c r="J10">
-        <f>F17</f>
+      <c r="K10">
+        <f>G17</f>
         <v>14576.4</v>
-      </c>
-      <c r="K10" t="b">
-        <v>1</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
       </c>
       <c r="M10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="E14" t="s">
         <v>40</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:16">
       <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>144</v>
       </c>
-      <c r="E15">
-        <f>D20*D15</f>
+      <c r="F15">
+        <f>E20*E15</f>
         <v>28.8</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="D16">
+    <row r="16" spans="1:16">
+      <c r="E16">
         <v>72</v>
       </c>
-      <c r="E16">
-        <f>D16*D20</f>
+      <c r="F16">
+        <f>E16*E20</f>
         <v>14.4</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="D17">
-        <f>I8</f>
+      <c r="E17">
+        <f>J8</f>
         <v>12147</v>
       </c>
-      <c r="E17">
-        <f>D17*$D$20</f>
+      <c r="F17">
+        <f>E17*$E$20</f>
         <v>2429.4</v>
       </c>
-      <c r="F17">
-        <f>D17+E17</f>
+      <c r="G17">
+        <f>E17+F17</f>
         <v>14576.4</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="H18" s="2"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:15">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="J19" s="3"/>
+      <c r="H19" s="2"/>
       <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="C20" t="s">
         <v>38</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>0.2</v>
       </c>
-      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="D23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="H20" s="2"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="E23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:15">
       <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:15">
       <c r="C27" s="2"/>
-      <c r="K27" s="10"/>
+      <c r="D27" s="2"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="N27" s="10"/>
+    </row>
+    <row r="28" spans="1:15">
       <c r="C28" s="2"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="10"/>
+      <c r="D28" s="2"/>
+      <c r="K28" s="4"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="J29" s="4"/>
+      <c r="N28" s="10"/>
+    </row>
+    <row r="29" spans="1:15">
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:15">
       <c r="C30" s="2"/>
-      <c r="I30" s="7" t="s">
+      <c r="D30" s="2"/>
+      <c r="J30" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="K30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>16</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1652,30 +1758,30 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>3</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>1</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <f>MEDIAN(B33:B35)</f>
         <v>53.415900000000001</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <f>_xlfn.STDEV.S(B33:B35)</f>
         <v>45.017725990790588</v>
       </c>
-      <c r="K31">
-        <f>I31-2*J31</f>
+      <c r="L31">
+        <f>J31-2*K31</f>
         <v>-36.619551981581175</v>
       </c>
-      <c r="L31">
-        <f>MEDIAN(I31+2*J31)</f>
+      <c r="M31">
+        <f>MEDIAN(J31+2*K31)</f>
         <v>143.45135198158118</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:15">
       <c r="A32" s="5">
         <v>4</v>
       </c>
@@ -1685,12 +1791,13 @@
       <c r="C32" s="5">
         <v>3.254219</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="5">
         <v>1</v>
       </c>
@@ -1700,12 +1807,13 @@
       <c r="C33" s="5">
         <v>43.227826999999998</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="5">
         <v>2</v>
       </c>
@@ -1715,11 +1823,12 @@
       <c r="C34" s="5">
         <v>9.6660740000000001</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:11">
       <c r="A35" s="6">
         <v>3</v>
       </c>
@@ -1729,15 +1838,16 @@
       <c r="C35" s="6">
         <v>11.303186999999999</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="K27:K28"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="M27:M28"/>
+    <mergeCell ref="N27:N28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>